<commit_message>
Comenzada idea de spawning en clusters, falta codigo
</commit_message>
<xml_diff>
--- a/Assets/.OtrosArchivos/Planificacion.xlsx
+++ b/Assets/.OtrosArchivos/Planificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos Unity\ShooterGame\Assets\.OtrosArchivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29CA6A03-B490-4BF6-A51A-BC20EBA7AC59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2493AB0-E271-4BE4-AA21-BB93F2B6C057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Nombre Enemigo</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Vida:</t>
+  </si>
+  <si>
+    <t>Daño Medio (de jugador)</t>
   </si>
 </sst>
 </file>
@@ -114,8 +117,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -399,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:J5"/>
+  <dimension ref="B1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,21 +419,23 @@
     <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -446,12 +454,15 @@
       <c r="G2" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="1"/>
+      <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -470,14 +481,17 @@
       <c r="G3">
         <v>10</v>
       </c>
-      <c r="I3" t="s">
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="J3" t="s">
         <v>8</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -496,15 +510,18 @@
       <c r="G4">
         <v>6</v>
       </c>
-      <c r="I4" t="s">
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="J4" t="s">
         <v>7</v>
       </c>
-      <c r="J4">
-        <f>J3*1.75</f>
+      <c r="K4">
+        <f>K3*1.75</f>
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -523,16 +540,19 @@
       <c r="G5">
         <v>20</v>
       </c>
-      <c r="I5" t="s">
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="J5" t="s">
         <v>13</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="J2:K2"/>
     <mergeCell ref="B1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Agregado spawneo de 3 tipos distintos de enemigos en clusters
</commit_message>
<xml_diff>
--- a/Assets/.OtrosArchivos/Planificacion.xlsx
+++ b/Assets/.OtrosArchivos/Planificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos Unity\ShooterGame\Assets\.OtrosArchivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2493AB0-E271-4BE4-AA21-BB93F2B6C057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24B179A-C000-462E-A53E-E949B030071E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -408,7 +408,7 @@
   <dimension ref="B1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,9 +416,9 @@
     <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3" bestFit="1" customWidth="1"/>
@@ -446,13 +446,13 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
         <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>2</v>
       </c>
       <c r="H2" t="s">
         <v>14</v>
@@ -473,13 +473,13 @@
         <v>0.75</v>
       </c>
       <c r="E3">
+        <v>0.25</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3">
         <v>40</v>
-      </c>
-      <c r="F3">
-        <v>0.25</v>
-      </c>
-      <c r="G3">
-        <v>10</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -502,13 +502,13 @@
         <v>2</v>
       </c>
       <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4">
         <v>40</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>6</v>
       </c>
       <c r="H4">
         <v>2</v>
@@ -532,13 +532,13 @@
         <v>5.5</v>
       </c>
       <c r="E5">
+        <v>3.5</v>
+      </c>
+      <c r="F5">
+        <v>20</v>
+      </c>
+      <c r="G5">
         <v>40</v>
-      </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
-      <c r="G5">
-        <v>20</v>
       </c>
       <c r="H5">
         <v>2</v>

</xml_diff>

<commit_message>
Actualizados paquetes, creadas hordas de enemigos
</commit_message>
<xml_diff>
--- a/Assets/.OtrosArchivos/Planificacion.xlsx
+++ b/Assets/.OtrosArchivos/Planificacion.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos Unity\ShooterGame\Assets\.OtrosArchivos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos Unity\ShootingGame\Assets\.OtrosArchivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24B179A-C000-462E-A53E-E949B030071E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755F41F6-1D25-467F-AAF9-29670F9DEEA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Enemigos" sheetId="1" r:id="rId1"/>
-    <sheet name="Armas y Balas" sheetId="2" r:id="rId2"/>
-    <sheet name="Oleadas" sheetId="3" r:id="rId3"/>
-    <sheet name="Boosts" sheetId="4" r:id="rId4"/>
+    <sheet name="Hordas" sheetId="5" r:id="rId1"/>
+    <sheet name="Enemigos" sheetId="1" r:id="rId2"/>
+    <sheet name="Armas y Balas" sheetId="2" r:id="rId3"/>
+    <sheet name="Oleadas" sheetId="3" r:id="rId4"/>
+    <sheet name="Boosts" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Nombre Enemigo</t>
   </si>
@@ -83,6 +84,18 @@
   <si>
     <t>Daño Medio (de jugador)</t>
   </si>
+  <si>
+    <t>Cant. total enemigos</t>
+  </si>
+  <si>
+    <t>Spawn cooldown</t>
+  </si>
+  <si>
+    <t>Num horda</t>
+  </si>
+  <si>
+    <t>Ataque final</t>
+  </si>
 </sst>
 </file>
 
@@ -105,7 +118,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -113,15 +126,56 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -404,10 +458,1861 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C729F9C4-C8B7-4D28-AA55-6528F102A68D}">
+  <dimension ref="A1:H142"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="6.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <f>4+B3</f>
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D34" si="0">4-0.2*(B3-1)+3.2*ROUNDDOWN(B3/16,0)</f>
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E50" si="1">IF(MOD(B3,4)=0,5*B3/4,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C66" si="2">4+B4</f>
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>3.8</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>3.6</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>3.4</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>3.2</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="5">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="5">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>2.8</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="5">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>2.5999999999999996</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="5">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>2.4</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="5">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="5">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="5">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="5">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>1.5999999999999996</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="5">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>1.4</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="5">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>1.1999999999999997</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="2">
+        <v>16</v>
+      </c>
+      <c r="C18" s="3">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="0"/>
+        <v>4.2</v>
+      </c>
+      <c r="E18" s="4">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="5">
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="5">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>3.8</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="5">
+        <v>19</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>3.6</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="5">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>3.4</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="5">
+        <v>21</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>3.2</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="5">
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="5">
+        <v>23</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>2.8</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="5">
+        <v>24</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>2.5999999999999996</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="5">
+        <v>25</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>2.3999999999999995</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="5">
+        <v>26</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="5">
+        <v>27</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="5">
+        <v>28</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="5">
+        <v>29</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>1.5999999999999996</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="5">
+        <v>30</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>1.3999999999999995</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="5">
+        <v>31</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="2">
+        <v>32</v>
+      </c>
+      <c r="C34" s="3">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="D34" s="3">
+        <f t="shared" si="0"/>
+        <v>4.2</v>
+      </c>
+      <c r="E34" s="4">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="5">
+        <v>33</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="D35">
+        <f t="shared" ref="D35:D66" si="3">4-0.2*(B35-1)+3.2*ROUNDDOWN(B35/16,0)</f>
+        <v>4</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="5">
+        <v>34</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="3"/>
+        <v>3.8</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="5">
+        <v>35</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="3"/>
+        <v>3.5999999999999996</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5">
+        <v>36</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="3"/>
+        <v>3.4000000000000004</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5">
+        <v>37</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="3"/>
+        <v>3.2</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5">
+        <v>38</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="5"/>
+      <c r="B41" s="5">
+        <v>39</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="3"/>
+        <v>2.8</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5">
+        <v>40</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="3"/>
+        <v>2.5999999999999996</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5">
+        <v>41</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="3"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F43" s="5"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="5"/>
+      <c r="B44" s="5">
+        <v>42</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="3"/>
+        <v>2.1999999999999993</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F44" s="5"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="5">
+        <v>43</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="5">
+        <v>44</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="3"/>
+        <v>1.8000000000000007</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B47" s="5">
+        <v>45</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="3"/>
+        <v>1.5999999999999996</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="5">
+        <v>46</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="3"/>
+        <v>1.4000000000000004</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="5">
+        <v>47</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="2"/>
+        <v>51</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="3"/>
+        <v>1.1999999999999993</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="2">
+        <v>48</v>
+      </c>
+      <c r="C50" s="3">
+        <f t="shared" si="2"/>
+        <v>52</v>
+      </c>
+      <c r="D50" s="3">
+        <f t="shared" si="3"/>
+        <v>4.2000000000000011</v>
+      </c>
+      <c r="E50" s="4">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B51" s="5">
+        <v>49</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="2"/>
+        <v>53</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E51" s="5">
+        <f t="shared" ref="E51:E66" si="4">IF(MOD(B51,4)=0,5*B51/4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B52" s="5">
+        <v>50</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="2"/>
+        <v>54</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="3"/>
+        <v>3.8000000000000007</v>
+      </c>
+      <c r="E52" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B53" s="5">
+        <v>51</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="3"/>
+        <v>3.6000000000000014</v>
+      </c>
+      <c r="E53" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B54" s="5">
+        <v>52</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="2"/>
+        <v>56</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="3"/>
+        <v>3.4000000000000004</v>
+      </c>
+      <c r="E54" s="5">
+        <f t="shared" si="4"/>
+        <v>65</v>
+      </c>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B55" s="5">
+        <v>53</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="2"/>
+        <v>57</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="3"/>
+        <v>3.2000000000000011</v>
+      </c>
+      <c r="E55" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B56" s="5">
+        <v>54</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E56" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B57" s="5">
+        <v>55</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="2"/>
+        <v>59</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="3"/>
+        <v>2.8000000000000007</v>
+      </c>
+      <c r="E57" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B58" s="5">
+        <v>56</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="3"/>
+        <v>2.6000000000000014</v>
+      </c>
+      <c r="E58" s="5">
+        <f t="shared" si="4"/>
+        <v>70</v>
+      </c>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B59" s="5">
+        <v>57</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="2"/>
+        <v>61</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="3"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="E59" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B60" s="5">
+        <v>58</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="2"/>
+        <v>62</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="3"/>
+        <v>2.2000000000000011</v>
+      </c>
+      <c r="E60" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B61" s="5">
+        <v>59</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="2"/>
+        <v>63</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E61" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B62" s="5">
+        <v>60</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="3"/>
+        <v>1.8000000000000007</v>
+      </c>
+      <c r="E62" s="5">
+        <f t="shared" si="4"/>
+        <v>75</v>
+      </c>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B63" s="5">
+        <v>61</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="2"/>
+        <v>65</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="3"/>
+        <v>1.6000000000000014</v>
+      </c>
+      <c r="E63" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B64" s="5">
+        <v>62</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="2"/>
+        <v>66</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="3"/>
+        <v>1.4000000000000004</v>
+      </c>
+      <c r="E64" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+    </row>
+    <row r="65" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="5">
+        <v>63</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="2"/>
+        <v>67</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="3"/>
+        <v>1.2000000000000011</v>
+      </c>
+      <c r="E65" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+    </row>
+    <row r="66" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="2">
+        <v>64</v>
+      </c>
+      <c r="C66" s="3">
+        <f t="shared" si="2"/>
+        <v>68</v>
+      </c>
+      <c r="D66" s="3">
+        <f t="shared" si="3"/>
+        <v>4.1999999999999993</v>
+      </c>
+      <c r="E66" s="4">
+        <f t="shared" si="4"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B68" s="5"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5"/>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+      <c r="G69" s="5"/>
+      <c r="H69" s="5"/>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
+      <c r="G71" s="5"/>
+      <c r="H71" s="5"/>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
+      <c r="G72" s="5"/>
+      <c r="H72" s="5"/>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5"/>
+      <c r="F73" s="5"/>
+      <c r="G73" s="5"/>
+      <c r="H73" s="5"/>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B74" s="5"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="5"/>
+      <c r="F74" s="5"/>
+      <c r="G74" s="5"/>
+      <c r="H74" s="5"/>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B75" s="5"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="5"/>
+      <c r="G75" s="5"/>
+      <c r="H75" s="5"/>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B76" s="5"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="5"/>
+      <c r="F76" s="5"/>
+      <c r="G76" s="5"/>
+      <c r="H76" s="5"/>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B77" s="5"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="5"/>
+      <c r="F77" s="5"/>
+      <c r="G77" s="5"/>
+      <c r="H77" s="5"/>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B78" s="5"/>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="5"/>
+      <c r="F78" s="5"/>
+      <c r="G78" s="5"/>
+      <c r="H78" s="5"/>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="5"/>
+      <c r="F79" s="5"/>
+      <c r="G79" s="5"/>
+      <c r="H79" s="5"/>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B80" s="5"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5"/>
+      <c r="F80" s="5"/>
+      <c r="G80" s="5"/>
+      <c r="H80" s="5"/>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B81" s="5"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5"/>
+      <c r="F81" s="5"/>
+      <c r="G81" s="5"/>
+      <c r="H81" s="5"/>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B82" s="5"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="5"/>
+      <c r="E82" s="5"/>
+      <c r="F82" s="5"/>
+      <c r="G82" s="5"/>
+      <c r="H82" s="5"/>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B83" s="5"/>
+      <c r="C83" s="5"/>
+      <c r="D83" s="5"/>
+      <c r="E83" s="5"/>
+      <c r="F83" s="5"/>
+      <c r="G83" s="5"/>
+      <c r="H83" s="5"/>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B84" s="5"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="5"/>
+      <c r="E84" s="5"/>
+      <c r="F84" s="5"/>
+      <c r="G84" s="5"/>
+      <c r="H84" s="5"/>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B85" s="5"/>
+      <c r="C85" s="5"/>
+      <c r="D85" s="5"/>
+      <c r="E85" s="5"/>
+      <c r="F85" s="5"/>
+      <c r="G85" s="5"/>
+      <c r="H85" s="5"/>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B86" s="5"/>
+      <c r="C86" s="5"/>
+      <c r="D86" s="5"/>
+      <c r="E86" s="5"/>
+      <c r="F86" s="5"/>
+      <c r="G86" s="5"/>
+      <c r="H86" s="5"/>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B87" s="5"/>
+      <c r="C87" s="5"/>
+      <c r="D87" s="5"/>
+      <c r="E87" s="5"/>
+      <c r="F87" s="5"/>
+      <c r="G87" s="5"/>
+      <c r="H87" s="5"/>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B88" s="5"/>
+      <c r="C88" s="5"/>
+      <c r="D88" s="5"/>
+      <c r="E88" s="5"/>
+      <c r="F88" s="5"/>
+      <c r="G88" s="5"/>
+      <c r="H88" s="5"/>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B89" s="5"/>
+      <c r="C89" s="5"/>
+      <c r="D89" s="5"/>
+      <c r="E89" s="5"/>
+      <c r="F89" s="5"/>
+      <c r="G89" s="5"/>
+      <c r="H89" s="5"/>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B90" s="5"/>
+      <c r="C90" s="5"/>
+      <c r="D90" s="5"/>
+      <c r="E90" s="5"/>
+      <c r="F90" s="5"/>
+      <c r="G90" s="5"/>
+      <c r="H90" s="5"/>
+    </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B91" s="5"/>
+      <c r="C91" s="5"/>
+      <c r="D91" s="5"/>
+      <c r="E91" s="5"/>
+      <c r="F91" s="5"/>
+      <c r="G91" s="5"/>
+      <c r="H91" s="5"/>
+    </row>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B92" s="5"/>
+      <c r="C92" s="5"/>
+      <c r="D92" s="5"/>
+      <c r="E92" s="5"/>
+      <c r="F92" s="5"/>
+      <c r="G92" s="5"/>
+      <c r="H92" s="5"/>
+    </row>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B93" s="5"/>
+      <c r="C93" s="5"/>
+      <c r="D93" s="5"/>
+      <c r="E93" s="5"/>
+      <c r="F93" s="5"/>
+      <c r="G93" s="5"/>
+      <c r="H93" s="5"/>
+    </row>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B94" s="5"/>
+      <c r="C94" s="5"/>
+      <c r="D94" s="5"/>
+      <c r="E94" s="5"/>
+      <c r="F94" s="5"/>
+      <c r="G94" s="5"/>
+      <c r="H94" s="5"/>
+    </row>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B95" s="5"/>
+      <c r="C95" s="5"/>
+      <c r="D95" s="5"/>
+      <c r="E95" s="5"/>
+      <c r="F95" s="5"/>
+      <c r="G95" s="5"/>
+      <c r="H95" s="5"/>
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B96" s="5"/>
+      <c r="C96" s="5"/>
+      <c r="D96" s="5"/>
+      <c r="E96" s="5"/>
+      <c r="F96" s="5"/>
+      <c r="G96" s="5"/>
+      <c r="H96" s="5"/>
+    </row>
+    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B97" s="5"/>
+      <c r="C97" s="5"/>
+      <c r="D97" s="5"/>
+      <c r="E97" s="5"/>
+      <c r="F97" s="5"/>
+      <c r="G97" s="5"/>
+      <c r="H97" s="5"/>
+    </row>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B98" s="5"/>
+      <c r="C98" s="5"/>
+      <c r="D98" s="5"/>
+      <c r="E98" s="5"/>
+      <c r="F98" s="5"/>
+      <c r="G98" s="5"/>
+      <c r="H98" s="5"/>
+    </row>
+    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B99" s="5"/>
+      <c r="C99" s="5"/>
+      <c r="D99" s="5"/>
+      <c r="E99" s="5"/>
+      <c r="F99" s="5"/>
+      <c r="G99" s="5"/>
+      <c r="H99" s="5"/>
+    </row>
+    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B100" s="5"/>
+      <c r="C100" s="5"/>
+      <c r="D100" s="5"/>
+      <c r="E100" s="5"/>
+      <c r="F100" s="5"/>
+      <c r="G100" s="5"/>
+      <c r="H100" s="5"/>
+    </row>
+    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B101" s="5"/>
+      <c r="C101" s="5"/>
+      <c r="D101" s="5"/>
+      <c r="E101" s="5"/>
+      <c r="F101" s="5"/>
+      <c r="G101" s="5"/>
+      <c r="H101" s="5"/>
+    </row>
+    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B102" s="5"/>
+      <c r="C102" s="5"/>
+      <c r="D102" s="5"/>
+      <c r="E102" s="5"/>
+      <c r="F102" s="5"/>
+      <c r="G102" s="5"/>
+      <c r="H102" s="5"/>
+    </row>
+    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B103" s="5"/>
+      <c r="C103" s="5"/>
+      <c r="D103" s="5"/>
+      <c r="E103" s="5"/>
+      <c r="F103" s="5"/>
+      <c r="G103" s="5"/>
+      <c r="H103" s="5"/>
+    </row>
+    <row r="104" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B104" s="5"/>
+      <c r="C104" s="5"/>
+      <c r="D104" s="5"/>
+      <c r="E104" s="5"/>
+      <c r="F104" s="5"/>
+      <c r="G104" s="5"/>
+      <c r="H104" s="5"/>
+    </row>
+    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B105" s="5"/>
+      <c r="C105" s="5"/>
+      <c r="D105" s="5"/>
+      <c r="E105" s="5"/>
+      <c r="F105" s="5"/>
+      <c r="G105" s="5"/>
+      <c r="H105" s="5"/>
+    </row>
+    <row r="106" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B106" s="5"/>
+      <c r="C106" s="5"/>
+      <c r="D106" s="5"/>
+      <c r="E106" s="5"/>
+      <c r="F106" s="5"/>
+      <c r="G106" s="5"/>
+      <c r="H106" s="5"/>
+    </row>
+    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B107" s="5"/>
+      <c r="C107" s="5"/>
+      <c r="D107" s="5"/>
+      <c r="E107" s="5"/>
+      <c r="F107" s="5"/>
+      <c r="G107" s="5"/>
+      <c r="H107" s="5"/>
+    </row>
+    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B108" s="5"/>
+      <c r="C108" s="5"/>
+      <c r="D108" s="5"/>
+      <c r="E108" s="5"/>
+      <c r="F108" s="5"/>
+      <c r="G108" s="5"/>
+      <c r="H108" s="5"/>
+    </row>
+    <row r="109" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B109" s="5"/>
+      <c r="C109" s="5"/>
+      <c r="D109" s="5"/>
+      <c r="E109" s="5"/>
+      <c r="F109" s="5"/>
+      <c r="G109" s="5"/>
+      <c r="H109" s="5"/>
+    </row>
+    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B110" s="5"/>
+      <c r="C110" s="5"/>
+      <c r="D110" s="5"/>
+      <c r="E110" s="5"/>
+      <c r="F110" s="5"/>
+      <c r="G110" s="5"/>
+      <c r="H110" s="5"/>
+    </row>
+    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B111" s="5"/>
+      <c r="C111" s="5"/>
+      <c r="D111" s="5"/>
+      <c r="E111" s="5"/>
+      <c r="F111" s="5"/>
+      <c r="G111" s="5"/>
+      <c r="H111" s="5"/>
+    </row>
+    <row r="112" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B112" s="5"/>
+      <c r="C112" s="5"/>
+      <c r="D112" s="5"/>
+      <c r="E112" s="5"/>
+      <c r="F112" s="5"/>
+      <c r="G112" s="5"/>
+      <c r="H112" s="5"/>
+    </row>
+    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B113" s="5"/>
+      <c r="C113" s="5"/>
+      <c r="D113" s="5"/>
+      <c r="E113" s="5"/>
+      <c r="F113" s="5"/>
+      <c r="G113" s="5"/>
+      <c r="H113" s="5"/>
+    </row>
+    <row r="114" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B114" s="5"/>
+      <c r="C114" s="5"/>
+      <c r="D114" s="5"/>
+      <c r="E114" s="5"/>
+      <c r="F114" s="5"/>
+      <c r="G114" s="5"/>
+      <c r="H114" s="5"/>
+    </row>
+    <row r="115" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B115" s="5"/>
+      <c r="C115" s="5"/>
+      <c r="D115" s="5"/>
+      <c r="E115" s="5"/>
+      <c r="F115" s="5"/>
+      <c r="G115" s="5"/>
+      <c r="H115" s="5"/>
+    </row>
+    <row r="116" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B116" s="5"/>
+      <c r="C116" s="5"/>
+      <c r="D116" s="5"/>
+      <c r="E116" s="5"/>
+      <c r="F116" s="5"/>
+      <c r="G116" s="5"/>
+      <c r="H116" s="5"/>
+    </row>
+    <row r="117" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B117" s="5"/>
+      <c r="C117" s="5"/>
+      <c r="D117" s="5"/>
+      <c r="E117" s="5"/>
+      <c r="F117" s="5"/>
+      <c r="G117" s="5"/>
+      <c r="H117" s="5"/>
+    </row>
+    <row r="118" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B118" s="5"/>
+      <c r="C118" s="5"/>
+      <c r="D118" s="5"/>
+      <c r="E118" s="5"/>
+      <c r="F118" s="5"/>
+      <c r="G118" s="5"/>
+      <c r="H118" s="5"/>
+    </row>
+    <row r="119" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B119" s="5"/>
+      <c r="C119" s="5"/>
+      <c r="D119" s="5"/>
+      <c r="E119" s="5"/>
+      <c r="F119" s="5"/>
+      <c r="G119" s="5"/>
+      <c r="H119" s="5"/>
+    </row>
+    <row r="120" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B120" s="5"/>
+      <c r="C120" s="5"/>
+      <c r="D120" s="5"/>
+      <c r="E120" s="5"/>
+      <c r="F120" s="5"/>
+      <c r="G120" s="5"/>
+      <c r="H120" s="5"/>
+    </row>
+    <row r="121" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B121" s="5"/>
+      <c r="C121" s="5"/>
+      <c r="D121" s="5"/>
+      <c r="E121" s="5"/>
+      <c r="F121" s="5"/>
+      <c r="G121" s="5"/>
+      <c r="H121" s="5"/>
+    </row>
+    <row r="122" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B122" s="5"/>
+      <c r="C122" s="5"/>
+      <c r="D122" s="5"/>
+      <c r="E122" s="5"/>
+      <c r="F122" s="5"/>
+      <c r="G122" s="5"/>
+      <c r="H122" s="5"/>
+    </row>
+    <row r="123" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B123" s="5"/>
+      <c r="C123" s="5"/>
+      <c r="D123" s="5"/>
+      <c r="E123" s="5"/>
+      <c r="F123" s="5"/>
+      <c r="G123" s="5"/>
+      <c r="H123" s="5"/>
+    </row>
+    <row r="124" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B124" s="5"/>
+      <c r="C124" s="5"/>
+      <c r="D124" s="5"/>
+      <c r="E124" s="5"/>
+      <c r="F124" s="5"/>
+      <c r="G124" s="5"/>
+      <c r="H124" s="5"/>
+    </row>
+    <row r="125" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B125" s="5"/>
+      <c r="C125" s="5"/>
+      <c r="D125" s="5"/>
+      <c r="E125" s="5"/>
+      <c r="F125" s="5"/>
+      <c r="G125" s="5"/>
+      <c r="H125" s="5"/>
+    </row>
+    <row r="126" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B126" s="5"/>
+      <c r="C126" s="5"/>
+      <c r="D126" s="5"/>
+      <c r="E126" s="5"/>
+      <c r="F126" s="5"/>
+      <c r="G126" s="5"/>
+      <c r="H126" s="5"/>
+    </row>
+    <row r="127" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B127" s="5"/>
+      <c r="C127" s="5"/>
+      <c r="D127" s="5"/>
+      <c r="E127" s="5"/>
+      <c r="F127" s="5"/>
+      <c r="G127" s="5"/>
+      <c r="H127" s="5"/>
+    </row>
+    <row r="128" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B128" s="5"/>
+      <c r="C128" s="5"/>
+      <c r="D128" s="5"/>
+      <c r="E128" s="5"/>
+      <c r="F128" s="5"/>
+      <c r="G128" s="5"/>
+      <c r="H128" s="5"/>
+    </row>
+    <row r="129" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B129" s="5"/>
+      <c r="C129" s="5"/>
+      <c r="D129" s="5"/>
+      <c r="E129" s="5"/>
+      <c r="F129" s="5"/>
+      <c r="G129" s="5"/>
+      <c r="H129" s="5"/>
+    </row>
+    <row r="130" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B130" s="5"/>
+      <c r="C130" s="5"/>
+      <c r="D130" s="5"/>
+      <c r="E130" s="5"/>
+      <c r="F130" s="5"/>
+      <c r="G130" s="5"/>
+      <c r="H130" s="5"/>
+    </row>
+    <row r="131" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B131" s="5"/>
+      <c r="C131" s="5"/>
+      <c r="D131" s="5"/>
+      <c r="E131" s="5"/>
+      <c r="F131" s="5"/>
+      <c r="G131" s="5"/>
+      <c r="H131" s="5"/>
+    </row>
+    <row r="132" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B132" s="5"/>
+      <c r="C132" s="5"/>
+      <c r="D132" s="5"/>
+      <c r="E132" s="5"/>
+      <c r="F132" s="5"/>
+      <c r="G132" s="5"/>
+      <c r="H132" s="5"/>
+    </row>
+    <row r="133" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B133" s="5"/>
+      <c r="C133" s="5"/>
+      <c r="D133" s="5"/>
+      <c r="E133" s="5"/>
+      <c r="F133" s="5"/>
+      <c r="G133" s="5"/>
+      <c r="H133" s="5"/>
+    </row>
+    <row r="134" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B134" s="5"/>
+      <c r="C134" s="5"/>
+      <c r="D134" s="5"/>
+      <c r="E134" s="5"/>
+      <c r="F134" s="5"/>
+      <c r="G134" s="5"/>
+      <c r="H134" s="5"/>
+    </row>
+    <row r="135" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B135" s="5"/>
+      <c r="C135" s="5"/>
+      <c r="D135" s="5"/>
+      <c r="E135" s="5"/>
+      <c r="F135" s="5"/>
+      <c r="G135" s="5"/>
+      <c r="H135" s="5"/>
+    </row>
+    <row r="136" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B136" s="5"/>
+      <c r="C136" s="5"/>
+      <c r="D136" s="5"/>
+      <c r="E136" s="5"/>
+      <c r="F136" s="5"/>
+      <c r="G136" s="5"/>
+      <c r="H136" s="5"/>
+    </row>
+    <row r="137" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B137" s="5"/>
+      <c r="C137" s="5"/>
+      <c r="D137" s="5"/>
+      <c r="E137" s="5"/>
+      <c r="F137" s="5"/>
+      <c r="G137" s="5"/>
+      <c r="H137" s="5"/>
+    </row>
+    <row r="138" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B138" s="5"/>
+      <c r="C138" s="5"/>
+      <c r="D138" s="5"/>
+      <c r="E138" s="5"/>
+      <c r="F138" s="5"/>
+      <c r="G138" s="5"/>
+      <c r="H138" s="5"/>
+    </row>
+    <row r="139" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B139" s="5"/>
+      <c r="C139" s="5"/>
+      <c r="D139" s="5"/>
+      <c r="E139" s="5"/>
+      <c r="F139" s="5"/>
+      <c r="G139" s="5"/>
+      <c r="H139" s="5"/>
+    </row>
+    <row r="140" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B140" s="5"/>
+      <c r="C140" s="5"/>
+      <c r="D140" s="5"/>
+      <c r="E140" s="5"/>
+      <c r="F140" s="5"/>
+      <c r="G140" s="5"/>
+      <c r="H140" s="5"/>
+    </row>
+    <row r="141" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B141" s="5"/>
+      <c r="C141" s="5"/>
+      <c r="D141" s="5"/>
+      <c r="E141" s="5"/>
+      <c r="F141" s="5"/>
+      <c r="G141" s="5"/>
+      <c r="H141" s="5"/>
+    </row>
+    <row r="142" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B142" s="5"/>
+      <c r="C142" s="5"/>
+      <c r="D142" s="5"/>
+      <c r="E142" s="5"/>
+      <c r="F142" s="5"/>
+      <c r="G142" s="5"/>
+      <c r="H142" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -425,14 +2330,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
@@ -457,10 +2362,10 @@
       <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="2"/>
+      <c r="K2" s="6"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -559,7 +2464,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73D5280B-874A-4A6A-A841-210729259A8F}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -571,7 +2476,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6A290EC-C51C-4827-A65C-692597978BB6}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -585,7 +2490,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E494A29-76C6-4EFE-B574-43E87E37219A}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Actualizada navmesh, creado spawning random de tipos de enemigos y cantidad
</commit_message>
<xml_diff>
--- a/Assets/.OtrosArchivos/Planificacion.xlsx
+++ b/Assets/.OtrosArchivos/Planificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos Unity\ShootingGame\Assets\.OtrosArchivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755F41F6-1D25-467F-AAF9-29670F9DEEA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0268B042-6DC2-40CC-BFA2-EDACBEADC741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Nombre Enemigo</t>
   </si>
@@ -85,16 +85,31 @@
     <t>Daño Medio (de jugador)</t>
   </si>
   <si>
-    <t>Cant. total enemigos</t>
+    <t>Tipo enemigo</t>
   </si>
   <si>
-    <t>Spawn cooldown</t>
+    <t>Cantidad spawneada</t>
   </si>
   <si>
-    <t>Num horda</t>
+    <t>Normal</t>
   </si>
   <si>
-    <t>Ataque final</t>
+    <t>Fast</t>
+  </si>
+  <si>
+    <t>Slow</t>
+  </si>
+  <si>
+    <t>Horda</t>
+  </si>
+  <si>
+    <t>Enemigos</t>
+  </si>
+  <si>
+    <t>Cooldown</t>
+  </si>
+  <si>
+    <t>Final Attack</t>
   </si>
 </sst>
 </file>
@@ -118,7 +133,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -163,11 +178,117 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -176,8 +297,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -459,1176 +638,2658 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C729F9C4-C8B7-4D28-AA55-6528F102A68D}">
-  <dimension ref="A1:H142"/>
+  <dimension ref="A1:Z142"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="11" width="7.5703125" customWidth="1"/>
+    <col min="17" max="20" width="7.28515625" customWidth="1"/>
+    <col min="24" max="24" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
+    <row r="1" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="29"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="29"/>
+      <c r="K2" s="30"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+    </row>
+    <row r="3" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="31"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3">
+      <c r="H3" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="22">
         <v>1</v>
       </c>
-      <c r="C3">
-        <f>4+B3</f>
+      <c r="J3" s="23">
+        <v>2</v>
+      </c>
+      <c r="K3" s="24">
+        <v>3</v>
+      </c>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="5"/>
+      <c r="Z3" s="5"/>
+    </row>
+    <row r="4" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <f>4+B4</f>
         <v>5</v>
       </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D34" si="0">4-0.2*(B3-1)+3.2*ROUNDDOWN(B3/16,0)</f>
+      <c r="D4">
+        <f t="shared" ref="D4:D35" si="0">4-0.2*(B4-1)+3.2*ROUNDDOWN(B4/16,0)</f>
         <v>4</v>
       </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E50" si="1">IF(MOD(B3,4)=0,5*B3/4,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4">
+      <c r="E4">
+        <f t="shared" ref="E4:E51" si="1">IF(MOD(B4,4)=0,5*B4/4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="7">
+        <f>(B4-1)*5</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="8">
+        <f>100-(B4-1)*5</f>
+        <v>100</v>
+      </c>
+      <c r="H4" s="9">
+        <v>0</v>
+      </c>
+      <c r="I4" s="8">
+        <f>95-(B4-1)*5</f>
+        <v>95</v>
+      </c>
+      <c r="J4" s="19">
+        <f>B4*4</f>
+        <v>4</v>
+      </c>
+      <c r="K4" s="20">
+        <f>B4</f>
+        <v>1</v>
+      </c>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="5"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="5"/>
+      <c r="Z4" s="5"/>
+    </row>
+    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B5">
         <v>2</v>
       </c>
-      <c r="C4">
-        <f t="shared" ref="C4:C66" si="2">4+B4</f>
+      <c r="C5">
+        <f t="shared" ref="C5:C67" si="2">4+B5</f>
         <v>6</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <f t="shared" si="0"/>
         <v>3.8</v>
       </c>
-      <c r="E4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5">
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F5" s="10">
+        <f t="shared" ref="F5:F10" si="3">(B5-1)*5</f>
+        <v>5</v>
+      </c>
+      <c r="G5" s="5">
+        <f t="shared" ref="G5:G13" si="4">100-(B5-1)*5</f>
+        <v>95</v>
+      </c>
+      <c r="H5" s="11">
+        <v>0</v>
+      </c>
+      <c r="I5" s="5">
+        <f t="shared" ref="I5:I21" si="5">95-(B5-1)*5</f>
+        <v>90</v>
+      </c>
+      <c r="J5" s="5">
+        <f t="shared" ref="J5:J9" si="6">B5*4</f>
+        <v>8</v>
+      </c>
+      <c r="K5" s="11">
+        <f t="shared" ref="K5:K9" si="7">B5</f>
+        <v>2</v>
+      </c>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="5"/>
+      <c r="Z5" s="5"/>
+    </row>
+    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B6">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <f t="shared" si="0"/>
         <v>3.6</v>
       </c>
-      <c r="E5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6">
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="10">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="G6" s="5">
+        <f t="shared" si="4"/>
+        <v>90</v>
+      </c>
+      <c r="H6" s="11">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
+        <f t="shared" si="5"/>
+        <v>85</v>
+      </c>
+      <c r="J6" s="5">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="K6" s="11">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
+      <c r="Z6" s="5"/>
+    </row>
+    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B7">
         <v>4</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <f t="shared" si="0"/>
         <v>3.4</v>
       </c>
-      <c r="E6">
+      <c r="E7">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7">
+      <c r="F7" s="10">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="G7" s="5">
+        <f t="shared" si="4"/>
+        <v>85</v>
+      </c>
+      <c r="H7" s="15">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5">
+        <f t="shared" si="5"/>
+        <v>80</v>
+      </c>
+      <c r="J7" s="5">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="K7" s="11">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
+      <c r="Z7" s="5"/>
+    </row>
+    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B8">
         <v>5</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="D7">
+      <c r="D8">
         <f t="shared" si="0"/>
         <v>3.2</v>
       </c>
-      <c r="E7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="5">
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="10">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="G8" s="5">
+        <f t="shared" si="4"/>
+        <v>80</v>
+      </c>
+      <c r="H8" s="15">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
+        <f t="shared" si="5"/>
+        <v>75</v>
+      </c>
+      <c r="J8" s="5">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="K8" s="11">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
+      <c r="Z8" s="5"/>
+    </row>
+    <row r="9" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="5">
         <v>6</v>
       </c>
-      <c r="C8">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="D8">
+      <c r="C9">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="D9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="5">
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="10">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="G9" s="5">
+        <f t="shared" si="4"/>
+        <v>75</v>
+      </c>
+      <c r="H9" s="15">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5">
+        <f t="shared" si="5"/>
+        <v>70</v>
+      </c>
+      <c r="J9" s="5">
+        <f t="shared" si="6"/>
+        <v>24</v>
+      </c>
+      <c r="K9" s="11">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="5"/>
+      <c r="Z9" s="5"/>
+    </row>
+    <row r="10" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="5">
         <v>7</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="D9">
+      <c r="D10">
         <f t="shared" si="0"/>
         <v>2.8</v>
       </c>
-      <c r="E9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="5">
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="12">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="G10" s="13">
+        <f t="shared" si="4"/>
+        <v>70</v>
+      </c>
+      <c r="H10" s="18">
+        <v>0</v>
+      </c>
+      <c r="I10" s="7">
+        <f t="shared" si="5"/>
+        <v>65</v>
+      </c>
+      <c r="J10" s="8">
+        <v>25</v>
+      </c>
+      <c r="K10" s="9">
+        <f>K9+4</f>
+        <v>10</v>
+      </c>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="5"/>
+    </row>
+    <row r="11" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B11" s="5">
         <v>8</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="D10">
+      <c r="D11">
         <f t="shared" si="0"/>
         <v>2.5999999999999996</v>
       </c>
-      <c r="E10">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="5">
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="F11" s="7">
+        <v>35</v>
+      </c>
+      <c r="G11" s="8">
+        <f t="shared" si="4"/>
+        <v>65</v>
+      </c>
+      <c r="H11" s="19">
+        <v>0</v>
+      </c>
+      <c r="I11" s="10">
+        <f t="shared" si="5"/>
+        <v>60</v>
+      </c>
+      <c r="J11" s="6">
+        <v>25</v>
+      </c>
+      <c r="K11" s="11">
+        <f t="shared" ref="K11:K20" si="8">K10+5</f>
+        <v>15</v>
+      </c>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="5"/>
+    </row>
+    <row r="12" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B12" s="5">
         <v>9</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="D11">
+      <c r="D12">
         <f t="shared" si="0"/>
         <v>2.4</v>
       </c>
-      <c r="E11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="5">
-        <v>10</v>
-      </c>
-      <c r="C12">
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="10">
+        <f>F11</f>
+        <v>35</v>
+      </c>
+      <c r="G12" s="5">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+      <c r="H12" s="5">
+        <f>(B12-8)*5</f>
+        <v>5</v>
+      </c>
+      <c r="I12" s="10">
+        <f t="shared" si="5"/>
+        <v>55</v>
+      </c>
+      <c r="J12" s="6">
+        <v>25</v>
+      </c>
+      <c r="K12" s="11">
+        <f t="shared" si="8"/>
+        <v>20</v>
+      </c>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="5"/>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="5"/>
+      <c r="Z12" s="5"/>
+    </row>
+    <row r="13" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="5">
+        <v>10</v>
+      </c>
+      <c r="C13">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="D12">
+      <c r="D13">
         <f t="shared" si="0"/>
         <v>2.2000000000000002</v>
       </c>
-      <c r="E12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="5">
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="12">
+        <f t="shared" ref="F13:F14" si="9">F12</f>
+        <v>35</v>
+      </c>
+      <c r="G13" s="13">
+        <f t="shared" si="4"/>
+        <v>55</v>
+      </c>
+      <c r="H13" s="13">
+        <f t="shared" ref="H13" si="10">(B13-8)*5</f>
+        <v>10</v>
+      </c>
+      <c r="I13" s="10">
+        <f t="shared" si="5"/>
+        <v>50</v>
+      </c>
+      <c r="J13" s="6">
+        <v>25</v>
+      </c>
+      <c r="K13" s="11">
+        <f t="shared" si="8"/>
+        <v>25</v>
+      </c>
+      <c r="M13" s="17"/>
+      <c r="N13" s="14"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="5"/>
+      <c r="Z13" s="5"/>
+    </row>
+    <row r="14" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B14" s="5">
         <v>11</v>
       </c>
-      <c r="C13">
-        <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="D13">
+      <c r="C14">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="D14">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="5">
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="5">
+        <f t="shared" si="9"/>
+        <v>35</v>
+      </c>
+      <c r="G14" s="5">
+        <v>50</v>
+      </c>
+      <c r="H14" s="5">
+        <v>15</v>
+      </c>
+      <c r="I14" s="10">
+        <f t="shared" si="5"/>
+        <v>45</v>
+      </c>
+      <c r="J14" s="6">
+        <v>25</v>
+      </c>
+      <c r="K14" s="11">
+        <f t="shared" si="8"/>
+        <v>30</v>
+      </c>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+    </row>
+    <row r="15" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B15" s="5">
         <v>12</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="D14">
+      <c r="D15">
         <f t="shared" si="0"/>
         <v>1.7999999999999998</v>
       </c>
-      <c r="E14">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="5">
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="F15" s="5">
+        <v>35</v>
+      </c>
+      <c r="G15" s="5">
+        <v>50</v>
+      </c>
+      <c r="H15" s="5">
+        <v>15</v>
+      </c>
+      <c r="I15" s="10">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="J15" s="6">
+        <v>25</v>
+      </c>
+      <c r="K15" s="11">
+        <f t="shared" si="8"/>
+        <v>35</v>
+      </c>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+    </row>
+    <row r="16" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B16" s="5">
         <v>13</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="D15">
+      <c r="D16">
         <f t="shared" si="0"/>
         <v>1.5999999999999996</v>
       </c>
-      <c r="E15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="5">
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="5">
+        <v>35</v>
+      </c>
+      <c r="G16" s="5">
+        <v>50</v>
+      </c>
+      <c r="H16" s="5">
+        <v>15</v>
+      </c>
+      <c r="I16" s="10">
+        <f t="shared" si="5"/>
+        <v>35</v>
+      </c>
+      <c r="J16" s="6">
+        <v>25</v>
+      </c>
+      <c r="K16" s="11">
+        <f t="shared" si="8"/>
+        <v>40</v>
+      </c>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="5">
         <v>14</v>
       </c>
-      <c r="C16">
+      <c r="C17">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="D16">
+      <c r="D17">
         <f t="shared" si="0"/>
         <v>1.4</v>
       </c>
-      <c r="E16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="5">
-        <v>15</v>
-      </c>
-      <c r="C17">
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="5">
+        <v>35</v>
+      </c>
+      <c r="G17" s="5">
+        <v>50</v>
+      </c>
+      <c r="H17" s="5">
+        <v>15</v>
+      </c>
+      <c r="I17" s="10">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="J17" s="6">
+        <v>25</v>
+      </c>
+      <c r="K17" s="11">
+        <f t="shared" si="8"/>
+        <v>45</v>
+      </c>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+    </row>
+    <row r="18" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="5">
+        <v>15</v>
+      </c>
+      <c r="C18">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <f t="shared" si="0"/>
         <v>1.1999999999999997</v>
       </c>
-      <c r="E17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="2">
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="5">
+        <v>35</v>
+      </c>
+      <c r="G18" s="5">
+        <v>50</v>
+      </c>
+      <c r="H18" s="5">
+        <v>15</v>
+      </c>
+      <c r="I18" s="10">
+        <f t="shared" si="5"/>
+        <v>25</v>
+      </c>
+      <c r="J18" s="6">
+        <v>25</v>
+      </c>
+      <c r="K18" s="11">
+        <f t="shared" si="8"/>
+        <v>50</v>
+      </c>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+    </row>
+    <row r="19" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="2">
         <v>16</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C19" s="3">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D19" s="3">
         <f t="shared" si="0"/>
         <v>4.2</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E19" s="3">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="5">
+      <c r="F19" s="5">
+        <v>35</v>
+      </c>
+      <c r="G19" s="5">
+        <v>50</v>
+      </c>
+      <c r="H19" s="5">
+        <v>15</v>
+      </c>
+      <c r="I19" s="10">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="J19" s="6">
+        <v>25</v>
+      </c>
+      <c r="K19" s="11">
+        <f t="shared" si="8"/>
+        <v>55</v>
+      </c>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B20" s="5">
         <v>17</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="D19">
+      <c r="D20">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="5">
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="5">
+        <v>35</v>
+      </c>
+      <c r="G20" s="5">
+        <v>50</v>
+      </c>
+      <c r="H20" s="5">
+        <v>15</v>
+      </c>
+      <c r="I20" s="10">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="J20" s="6">
+        <v>25</v>
+      </c>
+      <c r="K20" s="11">
+        <f t="shared" si="8"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="5">
         <v>18</v>
       </c>
-      <c r="C20">
+      <c r="C21">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="D20">
+      <c r="D21">
         <f t="shared" si="0"/>
         <v>3.8</v>
       </c>
-      <c r="E20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="5">
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="5">
+        <v>35</v>
+      </c>
+      <c r="G21" s="5">
+        <v>50</v>
+      </c>
+      <c r="H21" s="5">
+        <v>15</v>
+      </c>
+      <c r="I21" s="12">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J21" s="18">
+        <v>25</v>
+      </c>
+      <c r="K21" s="16">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B22" s="5">
         <v>19</v>
       </c>
-      <c r="C21">
+      <c r="C22">
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="D21">
+      <c r="D22">
         <f t="shared" si="0"/>
         <v>3.6</v>
       </c>
-      <c r="E21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="5">
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="5">
+        <v>35</v>
+      </c>
+      <c r="G22" s="5">
+        <v>50</v>
+      </c>
+      <c r="H22" s="5">
+        <v>15</v>
+      </c>
+      <c r="I22" s="6">
+        <f t="shared" ref="I22" si="11">I21</f>
+        <v>10</v>
+      </c>
+      <c r="J22" s="6">
+        <f t="shared" ref="J22" si="12">J21</f>
+        <v>25</v>
+      </c>
+      <c r="K22" s="6">
+        <f t="shared" ref="K22" si="13">K21</f>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B23" s="5">
         <v>20</v>
       </c>
-      <c r="C22">
+      <c r="C23">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="D22">
+      <c r="D23">
         <f t="shared" si="0"/>
         <v>3.4</v>
       </c>
-      <c r="E22">
-        <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="5">
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="F23" s="5">
+        <v>35</v>
+      </c>
+      <c r="G23" s="5">
+        <v>50</v>
+      </c>
+      <c r="H23" s="5">
+        <v>15</v>
+      </c>
+      <c r="I23" s="6">
+        <f t="shared" ref="I23:I67" si="14">I22</f>
+        <v>10</v>
+      </c>
+      <c r="J23" s="6">
+        <f t="shared" ref="J23:J67" si="15">J22</f>
+        <v>25</v>
+      </c>
+      <c r="K23" s="6">
+        <f t="shared" ref="K23:K67" si="16">K22</f>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B24" s="5">
         <v>21</v>
       </c>
-      <c r="C23">
-        <f t="shared" si="2"/>
-        <v>25</v>
-      </c>
-      <c r="D23">
+      <c r="C24">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="D24">
         <f t="shared" si="0"/>
         <v>3.2</v>
       </c>
-      <c r="E23">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="5">
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="5">
+        <v>35</v>
+      </c>
+      <c r="G24" s="5">
+        <v>50</v>
+      </c>
+      <c r="H24" s="5">
+        <v>15</v>
+      </c>
+      <c r="I24" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J24" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K24" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B25" s="5">
         <v>22</v>
       </c>
-      <c r="C24">
+      <c r="C25">
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="D24">
+      <c r="D25">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E24">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="5">
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="5">
+        <v>35</v>
+      </c>
+      <c r="G25" s="5">
+        <v>50</v>
+      </c>
+      <c r="H25" s="5">
+        <v>15</v>
+      </c>
+      <c r="I25" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J25" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K25" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B26" s="5">
         <v>23</v>
       </c>
-      <c r="C25">
+      <c r="C26">
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="D25">
+      <c r="D26">
         <f t="shared" si="0"/>
         <v>2.8</v>
       </c>
-      <c r="E25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="5">
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="5">
+        <v>35</v>
+      </c>
+      <c r="G26" s="5">
+        <v>50</v>
+      </c>
+      <c r="H26" s="5">
+        <v>15</v>
+      </c>
+      <c r="I26" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J26" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K26" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B27" s="5">
         <v>24</v>
       </c>
-      <c r="C26">
+      <c r="C27">
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="D26">
+      <c r="D27">
         <f t="shared" si="0"/>
         <v>2.5999999999999996</v>
       </c>
-      <c r="E26">
+      <c r="E27">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="5">
-        <v>25</v>
-      </c>
-      <c r="C27">
+      <c r="F27" s="5">
+        <v>35</v>
+      </c>
+      <c r="G27" s="5">
+        <v>50</v>
+      </c>
+      <c r="H27" s="5">
+        <v>15</v>
+      </c>
+      <c r="I27" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J27" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K27" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B28" s="5">
+        <v>25</v>
+      </c>
+      <c r="C28">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="D27">
+      <c r="D28">
         <f t="shared" si="0"/>
         <v>2.3999999999999995</v>
       </c>
-      <c r="E27">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="5">
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="5">
+        <v>35</v>
+      </c>
+      <c r="G28" s="5">
+        <v>50</v>
+      </c>
+      <c r="H28" s="5">
+        <v>15</v>
+      </c>
+      <c r="I28" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J28" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K28" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B29" s="5">
         <v>26</v>
       </c>
-      <c r="C28">
+      <c r="C29">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="D28">
+      <c r="D29">
         <f t="shared" si="0"/>
         <v>2.2000000000000002</v>
       </c>
-      <c r="E28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="5">
+      <c r="E29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="5">
+        <v>35</v>
+      </c>
+      <c r="G29" s="5">
+        <v>50</v>
+      </c>
+      <c r="H29" s="5">
+        <v>15</v>
+      </c>
+      <c r="I29" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J29" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K29" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B30" s="5">
         <v>27</v>
       </c>
-      <c r="C29">
+      <c r="C30">
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="D29">
+      <c r="D30">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E29">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="5">
+      <c r="E30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="5">
+        <v>35</v>
+      </c>
+      <c r="G30" s="5">
+        <v>50</v>
+      </c>
+      <c r="H30" s="5">
+        <v>15</v>
+      </c>
+      <c r="I30" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J30" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K30" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B31" s="5">
         <v>28</v>
       </c>
-      <c r="C30">
+      <c r="C31">
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="D30">
+      <c r="D31">
         <f t="shared" si="0"/>
         <v>1.7999999999999998</v>
       </c>
-      <c r="E30">
-        <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="5">
+      <c r="E31">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="F31" s="5">
+        <v>35</v>
+      </c>
+      <c r="G31" s="5">
+        <v>50</v>
+      </c>
+      <c r="H31" s="5">
+        <v>15</v>
+      </c>
+      <c r="I31" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J31" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K31" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B32" s="5">
         <v>29</v>
       </c>
-      <c r="C31">
+      <c r="C32">
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="D31">
+      <c r="D32">
         <f t="shared" si="0"/>
         <v>1.5999999999999996</v>
       </c>
-      <c r="E31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="5">
+      <c r="E32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F32" s="5">
+        <v>35</v>
+      </c>
+      <c r="G32" s="5">
+        <v>50</v>
+      </c>
+      <c r="H32" s="5">
+        <v>15</v>
+      </c>
+      <c r="I32" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J32" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K32" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="5">
         <v>30</v>
       </c>
-      <c r="C32">
+      <c r="C33">
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="D32">
+      <c r="D33">
         <f t="shared" si="0"/>
         <v>1.3999999999999995</v>
       </c>
-      <c r="E32">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="5">
+      <c r="E33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F33" s="5">
+        <v>35</v>
+      </c>
+      <c r="G33" s="5">
+        <v>50</v>
+      </c>
+      <c r="H33" s="5">
+        <v>15</v>
+      </c>
+      <c r="I33" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J33" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K33" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="5">
         <v>31</v>
       </c>
-      <c r="C33">
-        <f t="shared" si="2"/>
-        <v>35</v>
-      </c>
-      <c r="D33">
+      <c r="C34">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="D34">
         <f t="shared" si="0"/>
         <v>1.2000000000000002</v>
       </c>
-      <c r="E33">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="2">
+      <c r="E34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F34" s="5">
+        <v>35</v>
+      </c>
+      <c r="G34" s="5">
+        <v>50</v>
+      </c>
+      <c r="H34" s="5">
+        <v>15</v>
+      </c>
+      <c r="I34" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J34" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K34" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="2">
         <v>32</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C35" s="3">
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D35" s="3">
         <f t="shared" si="0"/>
         <v>4.2</v>
       </c>
-      <c r="E34" s="4">
+      <c r="E35" s="4">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="5">
+      <c r="F35" s="5">
+        <v>35</v>
+      </c>
+      <c r="G35" s="5">
+        <v>50</v>
+      </c>
+      <c r="H35" s="5">
+        <v>15</v>
+      </c>
+      <c r="I35" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J35" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K35" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B36" s="5">
         <v>33</v>
       </c>
-      <c r="C35">
+      <c r="C36">
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
-      <c r="D35">
-        <f t="shared" ref="D35:D66" si="3">4-0.2*(B35-1)+3.2*ROUNDDOWN(B35/16,0)</f>
+      <c r="D36">
+        <f t="shared" ref="D36:D67" si="17">4-0.2*(B36-1)+3.2*ROUNDDOWN(B36/16,0)</f>
         <v>4</v>
       </c>
-      <c r="E35">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="5">
+      <c r="E36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F36" s="5">
+        <v>35</v>
+      </c>
+      <c r="G36" s="5">
+        <v>50</v>
+      </c>
+      <c r="H36" s="5">
+        <v>15</v>
+      </c>
+      <c r="I36" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J36" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K36" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="5">
         <v>34</v>
       </c>
-      <c r="C36">
+      <c r="C37">
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="D36">
-        <f t="shared" si="3"/>
+      <c r="D37">
+        <f t="shared" si="17"/>
         <v>3.8</v>
       </c>
-      <c r="E36">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="5">
-        <v>35</v>
-      </c>
-      <c r="C37">
-        <f t="shared" si="2"/>
-        <v>39</v>
-      </c>
-      <c r="D37">
-        <f t="shared" si="3"/>
-        <v>3.5999999999999996</v>
-      </c>
       <c r="E37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F37" s="5">
+        <v>35</v>
+      </c>
+      <c r="G37" s="5">
+        <v>50</v>
+      </c>
+      <c r="H37" s="5">
+        <v>15</v>
+      </c>
+      <c r="I37" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J37" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K37" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="5">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C38">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D38">
-        <f t="shared" si="3"/>
-        <v>3.4000000000000004</v>
+        <f t="shared" si="17"/>
+        <v>3.5999999999999996</v>
       </c>
       <c r="E38">
         <f t="shared" si="1"/>
-        <v>45</v>
-      </c>
-      <c r="F38" s="5"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F38" s="5">
+        <v>35</v>
+      </c>
+      <c r="G38" s="5">
+        <v>50</v>
+      </c>
+      <c r="H38" s="5">
+        <v>15</v>
+      </c>
+      <c r="I38" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J38" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K38" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="5">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C39">
         <f t="shared" si="2"/>
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D39">
-        <f t="shared" si="3"/>
-        <v>3.2</v>
+        <f t="shared" si="17"/>
+        <v>3.4000000000000004</v>
       </c>
       <c r="E39">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F39" s="5"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="F39" s="5">
+        <v>35</v>
+      </c>
+      <c r="G39" s="5">
+        <v>50</v>
+      </c>
+      <c r="H39" s="5">
+        <v>15</v>
+      </c>
+      <c r="I39" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J39" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K39" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="5">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C40">
         <f t="shared" si="2"/>
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D40">
-        <f t="shared" si="3"/>
-        <v>3</v>
+        <f t="shared" si="17"/>
+        <v>3.2</v>
       </c>
       <c r="E40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F40" s="5"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F40" s="5">
+        <v>35</v>
+      </c>
+      <c r="G40" s="5">
+        <v>50</v>
+      </c>
+      <c r="H40" s="5">
+        <v>15</v>
+      </c>
+      <c r="I40" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J40" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K40" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="5">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C41">
         <f t="shared" si="2"/>
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D41">
-        <f t="shared" si="3"/>
-        <v>2.8</v>
+        <f t="shared" si="17"/>
+        <v>3</v>
       </c>
       <c r="E41">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F41" s="5"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F41" s="5">
+        <v>35</v>
+      </c>
+      <c r="G41" s="5">
+        <v>50</v>
+      </c>
+      <c r="H41" s="5">
+        <v>15</v>
+      </c>
+      <c r="I41" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J41" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K41" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="B42" s="5">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C42">
         <f t="shared" si="2"/>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D42">
-        <f t="shared" si="3"/>
-        <v>2.5999999999999996</v>
+        <f t="shared" si="17"/>
+        <v>2.8</v>
       </c>
       <c r="E42">
         <f t="shared" si="1"/>
-        <v>50</v>
-      </c>
-      <c r="F42" s="5"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F42" s="5">
+        <v>35</v>
+      </c>
+      <c r="G42" s="5">
+        <v>50</v>
+      </c>
+      <c r="H42" s="5">
+        <v>15</v>
+      </c>
+      <c r="I42" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J42" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K42" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="5">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C43">
         <f t="shared" si="2"/>
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D43">
-        <f t="shared" si="3"/>
-        <v>2.4000000000000004</v>
+        <f t="shared" si="17"/>
+        <v>2.5999999999999996</v>
       </c>
       <c r="E43">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F43" s="5"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="F43" s="5">
+        <v>35</v>
+      </c>
+      <c r="G43" s="5">
+        <v>50</v>
+      </c>
+      <c r="H43" s="5">
+        <v>15</v>
+      </c>
+      <c r="I43" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J43" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K43" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="B44" s="5">
+        <v>41</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="17"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F44" s="5">
+        <v>35</v>
+      </c>
+      <c r="G44" s="5">
+        <v>50</v>
+      </c>
+      <c r="H44" s="5">
+        <v>15</v>
+      </c>
+      <c r="I44" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J44" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K44" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="5">
         <v>42</v>
       </c>
-      <c r="C44">
+      <c r="C45">
         <f t="shared" si="2"/>
         <v>46</v>
       </c>
-      <c r="D44">
-        <f t="shared" si="3"/>
+      <c r="D45">
+        <f t="shared" si="17"/>
         <v>2.1999999999999993</v>
       </c>
-      <c r="E44">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F44" s="5"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="5">
+      <c r="E45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F45" s="5">
+        <v>35</v>
+      </c>
+      <c r="G45" s="5">
+        <v>50</v>
+      </c>
+      <c r="H45" s="5">
+        <v>15</v>
+      </c>
+      <c r="I45" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J45" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K45" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B46" s="5">
         <v>43</v>
       </c>
-      <c r="C45">
+      <c r="C46">
         <f t="shared" si="2"/>
         <v>47</v>
       </c>
-      <c r="D45">
-        <f t="shared" si="3"/>
+      <c r="D46">
+        <f t="shared" si="17"/>
         <v>2</v>
       </c>
-      <c r="E45">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B46" s="5">
+      <c r="E46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F46" s="5">
+        <v>35</v>
+      </c>
+      <c r="G46" s="5">
+        <v>50</v>
+      </c>
+      <c r="H46" s="5">
+        <v>15</v>
+      </c>
+      <c r="I46" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J46" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K46" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B47" s="5">
         <v>44</v>
       </c>
-      <c r="C46">
+      <c r="C47">
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
-      <c r="D46">
-        <f t="shared" si="3"/>
+      <c r="D47">
+        <f t="shared" si="17"/>
         <v>1.8000000000000007</v>
       </c>
-      <c r="E46">
+      <c r="E47">
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B47" s="5">
+      <c r="F47" s="5">
+        <v>35</v>
+      </c>
+      <c r="G47" s="5">
+        <v>50</v>
+      </c>
+      <c r="H47" s="5">
+        <v>15</v>
+      </c>
+      <c r="I47" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J47" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K47" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B48" s="5">
         <v>45</v>
       </c>
-      <c r="C47">
+      <c r="C48">
         <f t="shared" si="2"/>
         <v>49</v>
       </c>
-      <c r="D47">
-        <f t="shared" si="3"/>
+      <c r="D48">
+        <f t="shared" si="17"/>
         <v>1.5999999999999996</v>
       </c>
-      <c r="E47">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B48" s="5">
+      <c r="E48">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F48" s="5">
+        <v>35</v>
+      </c>
+      <c r="G48" s="5">
+        <v>50</v>
+      </c>
+      <c r="H48" s="5">
+        <v>15</v>
+      </c>
+      <c r="I48" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J48" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K48" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B49" s="5">
         <v>46</v>
       </c>
-      <c r="C48">
-        <f t="shared" si="2"/>
-        <v>50</v>
-      </c>
-      <c r="D48">
-        <f t="shared" si="3"/>
+      <c r="C49">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="17"/>
         <v>1.4000000000000004</v>
       </c>
-      <c r="E48">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="5">
+      <c r="E49">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F49" s="5">
+        <v>35</v>
+      </c>
+      <c r="G49" s="5">
+        <v>50</v>
+      </c>
+      <c r="H49" s="5">
+        <v>15</v>
+      </c>
+      <c r="I49" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J49" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K49" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="5">
         <v>47</v>
       </c>
-      <c r="C49">
+      <c r="C50">
         <f t="shared" si="2"/>
         <v>51</v>
       </c>
-      <c r="D49">
-        <f t="shared" si="3"/>
+      <c r="D50">
+        <f t="shared" si="17"/>
         <v>1.1999999999999993</v>
       </c>
-      <c r="E49">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="2">
+      <c r="E50">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F50" s="5">
+        <v>35</v>
+      </c>
+      <c r="G50" s="5">
+        <v>50</v>
+      </c>
+      <c r="H50" s="5">
+        <v>15</v>
+      </c>
+      <c r="I50" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J50" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K50" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="51" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="2">
         <v>48</v>
       </c>
-      <c r="C50" s="3">
+      <c r="C51" s="3">
         <f t="shared" si="2"/>
         <v>52</v>
       </c>
-      <c r="D50" s="3">
-        <f t="shared" si="3"/>
+      <c r="D51" s="3">
+        <f t="shared" si="17"/>
         <v>4.2000000000000011</v>
       </c>
-      <c r="E50" s="4">
+      <c r="E51" s="4">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B51" s="5">
+      <c r="F51" s="5">
+        <v>35</v>
+      </c>
+      <c r="G51" s="5">
+        <v>50</v>
+      </c>
+      <c r="H51" s="5">
+        <v>15</v>
+      </c>
+      <c r="I51" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J51" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K51" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B52" s="5">
         <v>49</v>
       </c>
-      <c r="C51">
+      <c r="C52">
         <f t="shared" si="2"/>
         <v>53</v>
       </c>
-      <c r="D51">
-        <f t="shared" si="3"/>
+      <c r="D52">
+        <f t="shared" si="17"/>
         <v>4</v>
       </c>
-      <c r="E51" s="5">
-        <f t="shared" ref="E51:E66" si="4">IF(MOD(B51,4)=0,5*B51/4,0)</f>
-        <v>0</v>
-      </c>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B52" s="5">
-        <v>50</v>
-      </c>
-      <c r="C52">
+      <c r="E52" s="5">
+        <f t="shared" ref="E52:E67" si="18">IF(MOD(B52,4)=0,5*B52/4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F52" s="5">
+        <v>35</v>
+      </c>
+      <c r="G52" s="5">
+        <v>50</v>
+      </c>
+      <c r="H52" s="5">
+        <v>15</v>
+      </c>
+      <c r="I52" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J52" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K52" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B53" s="5">
+        <v>50</v>
+      </c>
+      <c r="C53">
         <f t="shared" si="2"/>
         <v>54</v>
       </c>
-      <c r="D52">
-        <f t="shared" si="3"/>
+      <c r="D53">
+        <f t="shared" si="17"/>
         <v>3.8000000000000007</v>
       </c>
-      <c r="E52" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="5">
+      <c r="E53" s="5">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="F53" s="5">
+        <v>35</v>
+      </c>
+      <c r="G53" s="5">
+        <v>50</v>
+      </c>
+      <c r="H53" s="5">
+        <v>15</v>
+      </c>
+      <c r="I53" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J53" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K53" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B54" s="5">
         <v>51</v>
       </c>
-      <c r="C53">
+      <c r="C54">
         <f t="shared" si="2"/>
         <v>55</v>
       </c>
-      <c r="D53">
-        <f t="shared" si="3"/>
+      <c r="D54">
+        <f t="shared" si="17"/>
         <v>3.6000000000000014</v>
       </c>
-      <c r="E53" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B54" s="5">
+      <c r="E54" s="5">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="F54" s="5">
+        <v>35</v>
+      </c>
+      <c r="G54" s="5">
+        <v>50</v>
+      </c>
+      <c r="H54" s="5">
+        <v>15</v>
+      </c>
+      <c r="I54" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J54" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K54" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B55" s="5">
         <v>52</v>
       </c>
-      <c r="C54">
+      <c r="C55">
         <f t="shared" si="2"/>
         <v>56</v>
       </c>
-      <c r="D54">
-        <f t="shared" si="3"/>
+      <c r="D55">
+        <f t="shared" si="17"/>
         <v>3.4000000000000004</v>
       </c>
-      <c r="E54" s="5">
-        <f t="shared" si="4"/>
-        <v>65</v>
-      </c>
-      <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B55" s="5">
+      <c r="E55" s="5">
+        <f t="shared" si="18"/>
+        <v>65</v>
+      </c>
+      <c r="F55" s="5">
+        <v>35</v>
+      </c>
+      <c r="G55" s="5">
+        <v>50</v>
+      </c>
+      <c r="H55" s="5">
+        <v>15</v>
+      </c>
+      <c r="I55" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J55" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K55" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B56" s="5">
         <v>53</v>
       </c>
-      <c r="C55">
+      <c r="C56">
         <f t="shared" si="2"/>
         <v>57</v>
       </c>
-      <c r="D55">
-        <f t="shared" si="3"/>
+      <c r="D56">
+        <f t="shared" si="17"/>
         <v>3.2000000000000011</v>
       </c>
-      <c r="E55" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F55" s="5"/>
-      <c r="G55" s="5"/>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B56" s="5">
+      <c r="E56" s="5">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="F56" s="5">
+        <v>35</v>
+      </c>
+      <c r="G56" s="5">
+        <v>50</v>
+      </c>
+      <c r="H56" s="5">
+        <v>15</v>
+      </c>
+      <c r="I56" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J56" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K56" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B57" s="5">
         <v>54</v>
       </c>
-      <c r="C56">
+      <c r="C57">
         <f t="shared" si="2"/>
         <v>58</v>
       </c>
-      <c r="D56">
-        <f t="shared" si="3"/>
+      <c r="D57">
+        <f t="shared" si="17"/>
         <v>3</v>
       </c>
-      <c r="E56" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F56" s="5"/>
-      <c r="G56" s="5"/>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B57" s="5">
+      <c r="E57" s="5">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="F57" s="5">
+        <v>35</v>
+      </c>
+      <c r="G57" s="5">
+        <v>50</v>
+      </c>
+      <c r="H57" s="5">
+        <v>15</v>
+      </c>
+      <c r="I57" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J57" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K57" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B58" s="5">
         <v>55</v>
       </c>
-      <c r="C57">
+      <c r="C58">
         <f t="shared" si="2"/>
         <v>59</v>
       </c>
-      <c r="D57">
-        <f t="shared" si="3"/>
+      <c r="D58">
+        <f t="shared" si="17"/>
         <v>2.8000000000000007</v>
       </c>
-      <c r="E57" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F57" s="5"/>
-      <c r="G57" s="5"/>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B58" s="5">
+      <c r="E58" s="5">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="F58" s="5">
+        <v>35</v>
+      </c>
+      <c r="G58" s="5">
+        <v>50</v>
+      </c>
+      <c r="H58" s="5">
+        <v>15</v>
+      </c>
+      <c r="I58" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J58" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K58" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B59" s="5">
         <v>56</v>
       </c>
-      <c r="C58">
+      <c r="C59">
         <f t="shared" si="2"/>
         <v>60</v>
       </c>
-      <c r="D58">
-        <f t="shared" si="3"/>
+      <c r="D59">
+        <f t="shared" si="17"/>
         <v>2.6000000000000014</v>
       </c>
-      <c r="E58" s="5">
-        <f t="shared" si="4"/>
+      <c r="E59" s="5">
+        <f t="shared" si="18"/>
         <v>70</v>
       </c>
-      <c r="F58" s="5"/>
-      <c r="G58" s="5"/>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B59" s="5">
+      <c r="F59" s="5">
+        <v>35</v>
+      </c>
+      <c r="G59" s="5">
+        <v>50</v>
+      </c>
+      <c r="H59" s="5">
+        <v>15</v>
+      </c>
+      <c r="I59" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J59" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K59" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B60" s="5">
         <v>57</v>
       </c>
-      <c r="C59">
+      <c r="C60">
         <f t="shared" si="2"/>
         <v>61</v>
       </c>
-      <c r="D59">
-        <f t="shared" si="3"/>
+      <c r="D60">
+        <f t="shared" si="17"/>
         <v>2.4000000000000004</v>
       </c>
-      <c r="E59" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F59" s="5"/>
-      <c r="G59" s="5"/>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B60" s="5">
+      <c r="E60" s="5">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="F60" s="5">
+        <v>35</v>
+      </c>
+      <c r="G60" s="5">
+        <v>50</v>
+      </c>
+      <c r="H60" s="5">
+        <v>15</v>
+      </c>
+      <c r="I60" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J60" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K60" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B61" s="5">
         <v>58</v>
       </c>
-      <c r="C60">
+      <c r="C61">
         <f t="shared" si="2"/>
         <v>62</v>
       </c>
-      <c r="D60">
-        <f t="shared" si="3"/>
+      <c r="D61">
+        <f t="shared" si="17"/>
         <v>2.2000000000000011</v>
       </c>
-      <c r="E60" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F60" s="5"/>
-      <c r="G60" s="5"/>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B61" s="5">
+      <c r="E61" s="5">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="F61" s="5">
+        <v>35</v>
+      </c>
+      <c r="G61" s="5">
+        <v>50</v>
+      </c>
+      <c r="H61" s="5">
+        <v>15</v>
+      </c>
+      <c r="I61" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J61" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K61" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B62" s="5">
         <v>59</v>
       </c>
-      <c r="C61">
+      <c r="C62">
         <f t="shared" si="2"/>
         <v>63</v>
       </c>
-      <c r="D61">
-        <f t="shared" si="3"/>
+      <c r="D62">
+        <f t="shared" si="17"/>
         <v>2</v>
       </c>
-      <c r="E61" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F61" s="5"/>
-      <c r="G61" s="5"/>
-    </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B62" s="5">
+      <c r="E62" s="5">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="F62" s="5">
+        <v>35</v>
+      </c>
+      <c r="G62" s="5">
+        <v>50</v>
+      </c>
+      <c r="H62" s="5">
+        <v>15</v>
+      </c>
+      <c r="I62" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J62" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K62" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B63" s="5">
         <v>60</v>
       </c>
-      <c r="C62">
+      <c r="C63">
         <f t="shared" si="2"/>
         <v>64</v>
       </c>
-      <c r="D62">
-        <f t="shared" si="3"/>
+      <c r="D63">
+        <f t="shared" si="17"/>
         <v>1.8000000000000007</v>
       </c>
-      <c r="E62" s="5">
-        <f t="shared" si="4"/>
+      <c r="E63" s="5">
+        <f t="shared" si="18"/>
         <v>75</v>
       </c>
-      <c r="F62" s="5"/>
-      <c r="G62" s="5"/>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B63" s="5">
+      <c r="F63" s="5">
+        <v>35</v>
+      </c>
+      <c r="G63" s="5">
+        <v>50</v>
+      </c>
+      <c r="H63" s="5">
+        <v>15</v>
+      </c>
+      <c r="I63" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J63" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K63" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B64" s="5">
         <v>61</v>
       </c>
-      <c r="C63">
-        <f t="shared" si="2"/>
-        <v>65</v>
-      </c>
-      <c r="D63">
-        <f t="shared" si="3"/>
+      <c r="C64">
+        <f t="shared" si="2"/>
+        <v>65</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="17"/>
         <v>1.6000000000000014</v>
       </c>
-      <c r="E63" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F63" s="5"/>
-      <c r="G63" s="5"/>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B64" s="5">
+      <c r="E64" s="5">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="F64" s="5">
+        <v>35</v>
+      </c>
+      <c r="G64" s="5">
+        <v>50</v>
+      </c>
+      <c r="H64" s="5">
+        <v>15</v>
+      </c>
+      <c r="I64" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J64" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K64" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B65" s="5">
         <v>62</v>
       </c>
-      <c r="C64">
+      <c r="C65">
         <f t="shared" si="2"/>
         <v>66</v>
       </c>
-      <c r="D64">
-        <f t="shared" si="3"/>
+      <c r="D65">
+        <f t="shared" si="17"/>
         <v>1.4000000000000004</v>
       </c>
-      <c r="E64" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F64" s="5"/>
-      <c r="G64" s="5"/>
-    </row>
-    <row r="65" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="5">
+      <c r="E65" s="5">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="F65" s="5">
+        <v>35</v>
+      </c>
+      <c r="G65" s="5">
+        <v>50</v>
+      </c>
+      <c r="H65" s="5">
+        <v>15</v>
+      </c>
+      <c r="I65" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J65" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K65" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="5">
         <v>63</v>
       </c>
-      <c r="C65">
+      <c r="C66">
         <f t="shared" si="2"/>
         <v>67</v>
       </c>
-      <c r="D65">
-        <f t="shared" si="3"/>
+      <c r="D66">
+        <f t="shared" si="17"/>
         <v>1.2000000000000011</v>
       </c>
-      <c r="E65" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F65" s="5"/>
-      <c r="G65" s="5"/>
-    </row>
-    <row r="66" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="2">
+      <c r="E66" s="5">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="F66" s="5">
+        <v>35</v>
+      </c>
+      <c r="G66" s="5">
+        <v>50</v>
+      </c>
+      <c r="H66" s="5">
+        <v>15</v>
+      </c>
+      <c r="I66" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J66" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K66" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="2">
         <v>64</v>
       </c>
-      <c r="C66" s="3">
+      <c r="C67" s="3">
         <f t="shared" si="2"/>
         <v>68</v>
       </c>
-      <c r="D66" s="3">
-        <f t="shared" si="3"/>
+      <c r="D67" s="3">
+        <f t="shared" si="17"/>
         <v>4.1999999999999993</v>
       </c>
-      <c r="E66" s="4">
-        <f t="shared" si="4"/>
+      <c r="E67" s="4">
+        <f t="shared" si="18"/>
         <v>80</v>
       </c>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="5"/>
-      <c r="G67" s="5"/>
-    </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F67" s="5">
+        <v>35</v>
+      </c>
+      <c r="G67" s="5">
+        <v>50</v>
+      </c>
+      <c r="H67" s="5">
+        <v>15</v>
+      </c>
+      <c r="I67" s="6">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="J67" s="6">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="K67" s="6">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
@@ -1637,7 +3298,7 @@
       <c r="G68" s="5"/>
       <c r="H68" s="5"/>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
@@ -1646,7 +3307,7 @@
       <c r="G69" s="5"/>
       <c r="H69" s="5"/>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
@@ -1655,7 +3316,7 @@
       <c r="G70" s="5"/>
       <c r="H70" s="5"/>
     </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
@@ -1664,7 +3325,7 @@
       <c r="G71" s="5"/>
       <c r="H71" s="5"/>
     </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
@@ -1673,7 +3334,7 @@
       <c r="G72" s="5"/>
       <c r="H72" s="5"/>
     </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
@@ -1682,7 +3343,7 @@
       <c r="G73" s="5"/>
       <c r="H73" s="5"/>
     </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
@@ -1691,7 +3352,7 @@
       <c r="G74" s="5"/>
       <c r="H74" s="5"/>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
@@ -1700,7 +3361,7 @@
       <c r="G75" s="5"/>
       <c r="H75" s="5"/>
     </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
@@ -1709,7 +3370,7 @@
       <c r="G76" s="5"/>
       <c r="H76" s="5"/>
     </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
@@ -1718,7 +3379,7 @@
       <c r="G77" s="5"/>
       <c r="H77" s="5"/>
     </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
@@ -1727,7 +3388,7 @@
       <c r="G78" s="5"/>
       <c r="H78" s="5"/>
     </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
@@ -1736,7 +3397,7 @@
       <c r="G79" s="5"/>
       <c r="H79" s="5"/>
     </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
@@ -2304,7 +3965,16 @@
       <c r="H142" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="C2:C3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2330,14 +4000,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
@@ -2362,10 +4032,10 @@
       <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="6"/>
+      <c r="J2" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="21"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">

</xml_diff>